<commit_message>
computed all except SD
</commit_message>
<xml_diff>
--- a/Document/wordsentenceCOUNTforENGLISH.xlsx
+++ b/Document/wordsentenceCOUNTforENGLISH.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="84">
   <si>
     <t>English1</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>ARA</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,12 +738,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.35289999999999999</v>
-      </c>
+      <c r="C3" s="2"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:9">
@@ -2674,8 +2672,46 @@
         <v>74</v>
       </c>
     </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B74">
+        <f>SUM(B3:B73)/68</f>
+        <v>0.14609852941176471</v>
+      </c>
+      <c r="C74" s="2">
+        <f>SUM(C3:C73)/68</f>
+        <v>0.41514411764705877</v>
+      </c>
+      <c r="D74">
+        <f>SUM(D3:D73)/68</f>
+        <v>0.47712794117647078</v>
+      </c>
+      <c r="E74" s="4">
+        <f>SUM(E3:E73)/68</f>
+        <v>0.12308823529411755</v>
+      </c>
+      <c r="F74">
+        <f>SUM(F3:F73)/68</f>
+        <v>9.09151470588235</v>
+      </c>
+      <c r="G74">
+        <f>SUM(G3:G73)/68</f>
+        <v>0.30998397058823529</v>
+      </c>
+      <c r="H74">
+        <f>SUM(H3:H73)/68</f>
+        <v>0.15616617647058822</v>
+      </c>
+      <c r="I74">
+        <f>SUM(I3:I73)/68</f>
+        <v>0.24654558823529424</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2683,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3537,7 +3573,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" si="0"/>
+        <f>C58/B58</f>
         <v>0.39285714285714285</v>
       </c>
     </row>

</xml_diff>